<commit_message>
Change test_path to test_divert
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestDocuments/whitebox-test-cases-g3.xlsx
+++ b/Documents/Testing/TestDocuments/whitebox-test-cases-g3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaitl\OneDrive\Documents\CANADA\SENECA\ALL COURSES\SEMESTER 2\SFT221\PROJECT\ms4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaitl\OneDrive\Documents\CANADA\SENECA\ALL COURSES\SEMESTER 2\SFT221\PROJECT\winter25-sft221-nee-3\Documents\Testing\TestDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24477BE9-F0A4-4A38-BEF4-829AF8199A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300F382B-BBEC-4333-9AE2-5A39717DAAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="137">
   <si>
     <t>ID</t>
   </si>
@@ -245,82 +245,6 @@
     <t>Returned map should display the base map with the yellow route (Y symbol).</t>
   </si>
   <si>
-    <t>test_path1</t>
-  </si>
-  <si>
-    <t>Verify if the a algorithm finds the shortest path from 1A to 5E.</t>
-  </si>
-  <si>
-    <t>1. Set starting point to 1A (office location). 
-2. Set destination to 5E.  
-3. Run the algorithm to calculate the path. 
-4. Verify the calculated path.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Starting Point: 1A
-Destination: 5E	</t>
-  </si>
-  <si>
-    <t>Shortest path: 1A → 2A → 3A → 4A → 5A → 5B → 5C → 5D → 5E.</t>
-  </si>
-  <si>
-    <t>test_path2</t>
-  </si>
-  <si>
-    <t>Verify if the algorithm finds the shortest path from 10K to 15P.</t>
-  </si>
-  <si>
-    <t>Starting Point: 10K
-Destination: 17L</t>
-  </si>
-  <si>
-    <t>1. Set starting point to 10K .
-2. Set destination to 17L.
-3. Run the algorithm to calculate the path.	
-4. Verify the calculated path.</t>
-  </si>
-  <si>
-    <t>Shortest path: 10K → 11K → 12K → 13K → 14K → 15K → 16K → 17K → 17L</t>
-  </si>
-  <si>
-    <t>test_path3</t>
-  </si>
-  <si>
-    <t>Verify if the algorithm detects an unreachable destination (e.g., blocked by buildings).</t>
-  </si>
-  <si>
-    <t>1. Set starting point to 6E
-2. Set destination to 2H (blocked by buildings)
-3. Run the algorithm to calculate the path.	
-4. Verify the system's response.</t>
-  </si>
-  <si>
-    <t>Destination unreachable. Package cannot be delivered / ERROR.</t>
-  </si>
-  <si>
-    <t>Starting Point: 6E
-Destination: 2H</t>
-  </si>
-  <si>
-    <t>test_path4</t>
-  </si>
-  <si>
-    <t>Verify if the algorithm handles a diversion path around a building.</t>
-  </si>
-  <si>
-    <t>Diversion path: 18V → 17V → 16V → 15V → 14V → 13V → 12V → 11V → 10V → 9V → 8V → 7V → 7W → 7X → 7Y .</t>
-  </si>
-  <si>
-    <t>Starting Point: 18v
-Destination: 7Y</t>
-  </si>
-  <si>
-    <t>1. Set starting point to 18V (blue route).
-2. Set destination to 7Y.
-3. Run the algorithm to calculate the path.
-4. Verify the calculated path.</t>
-  </si>
-  <si>
     <t>test_assign1</t>
   </si>
   <si>
@@ -589,6 +513,78 @@
 2. Enter package details: Weight = 500 kg, Size = 5 m³.
 3. Verify the system's response.
 </t>
+  </si>
+  <si>
+    <t>test_divert1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify if the divert function correctly calculates the diversion path for a valid shipment.</t>
+  </si>
+  <si>
+    <t>1. Initialize a map, a truck, and a valid shipment.
+2. Call the divert function with the shipment and truck.
+3. Verify the calculated diversion path.</t>
+  </si>
+  <si>
+    <t>Map: Valid grid with buildings and empty spaces.
+Truck: Route includes points like 11K, 10K, 9K, etc.
+Shipment: Weight = 500 kg, Size = 5 m³, Address = 8P.</t>
+  </si>
+  <si>
+    <t>Expected Result: Diversion path calculated (e.g., 11K → 10K → 9K → 8K → 8P).</t>
+  </si>
+  <si>
+    <t>test_divert2</t>
+  </si>
+  <si>
+    <t>Verify if the divert function returns -1 for an invalid shipment (invalid destination).</t>
+  </si>
+  <si>
+    <t>1. Initialize a map, a truck, and an invalid shipment (destination outside the map or not a building).
+2. Call the divert function with the shipment and truck.
+3. Verify the return value.</t>
+  </si>
+  <si>
+    <t>Map: Valid grid with buildings and empty spaces.
+Truck: Route includes points like 11K, 10K, 9K, etc.
+Shipment: Weight = 500 kg, Size = 5 m³, Address = 0A (invalid).</t>
+  </si>
+  <si>
+    <t>Expected Result: Return -1 (invalid shipment).</t>
+  </si>
+  <si>
+    <t>test_divert3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify if the divert function returns -1 when the destination is unreachable (blocked by buildings).</t>
+  </si>
+  <si>
+    <t>1. Initialize a map with buildings blocking the path to the destination.
+Initialize a truck and a valid shipment.
+2. Call the divert function with the shipment and truck.
+3. Verify the return value."</t>
+  </si>
+  <si>
+    <t>Map: Buildings block the path to the destination (e.g., 15Q).
+Truck: Route includes points like 11K, 10K, 9K, etc.
+Shipment: Weight = 500 kg, Size = 5 m³, Address = 15Q.</t>
+  </si>
+  <si>
+    <t>Expected Result: Return -1 (destination unreachable).</t>
+  </si>
+  <si>
+    <t>test_divert4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify if the divert function correctly prints the diversion path.</t>
+  </si>
+  <si>
+    <t>1. Initialize a map, a truck, and a valid shipment.
+2. Call the divert function with the shipment and truck.
+3. Verify the printed diversion path.</t>
+  </si>
+  <si>
+    <t>Expected Result: Printed diversion path (e.g., "divert 11K, 10K, 9K, 8K, 8P").</t>
   </si>
 </sst>
 </file>
@@ -650,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -666,12 +662,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -682,6 +672,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -970,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="103" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1024,7 +1033,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
@@ -1047,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
@@ -1070,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
@@ -1093,7 +1102,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1113,10 +1122,10 @@
         <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>1</v>
@@ -1125,7 +1134,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
@@ -1136,7 +1145,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>33</v>
@@ -1148,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
@@ -1159,10 +1168,10 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E9" s="2" t="b">
         <v>0</v>
@@ -1171,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
@@ -1182,10 +1191,10 @@
         <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="E10" s="2" t="b">
         <v>0</v>
@@ -1194,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1285,73 +1294,81 @@
       <c r="F16" s="5"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>71</v>
-      </c>
+    <row r="17" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -1364,16 +1381,16 @@
     </row>
     <row r="22" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="E22" s="2">
         <v>0</v>
@@ -1382,21 +1399,21 @@
         <v>0</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="E23" s="2">
         <v>1</v>
@@ -1405,21 +1422,21 @@
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="E24" s="2">
         <v>1</v>
@@ -1428,21 +1445,21 @@
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="E25" s="2">
         <v>-1</v>
@@ -1451,93 +1468,93 @@
         <v>-1</v>
       </c>
       <c r="G25" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
@@ -1548,84 +1565,84 @@
       <c r="F31" s="5"/>
       <c r="G31" s="6"/>
       <c r="H31" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="12"/>
+      <c r="A32" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="12"/>
+      <c r="A33" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="F34" s="11"/>
-      <c r="G34" s="12"/>
+      <c r="A34" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35" s="11"/>
-      <c r="G35" s="12"/>
+      <c r="A35" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>

</xml_diff>

<commit_message>
replaced addRoute with path
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestDocuments/whitebox-test-cases-g3.xlsx
+++ b/Documents/Testing/TestDocuments/whitebox-test-cases-g3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaitl\OneDrive\Documents\CANADA\SENECA\ALL COURSES\SEMESTER 2\SFT221\PROJECT\winter25-sft221-nee-3\Documents\Testing\TestDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300F382B-BBEC-4333-9AE2-5A39717DAAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7333C11E-D403-40AB-BD33-022566AA81B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -161,88 +161,80 @@
 map.squares[1][2] = 1</t>
   </si>
   <si>
-    <t>test_addRoute1</t>
-  </si>
-  <si>
-    <t>test_addRoute2</t>
-  </si>
-  <si>
-    <t>test_addRoute3</t>
-  </si>
-  <si>
-    <t>test_addRoute4</t>
-  </si>
-  <si>
-    <t>Test that the function prints nothing when two routes are incorrectly passed instead of one map and one route.</t>
-  </si>
-  <si>
-    <t>Test that the function properly adds the blue route to the map</t>
-  </si>
-  <si>
-    <t>Test that the function properly adds the yellow route to the map</t>
-  </si>
-  <si>
-    <t>Test that the function properly adds the green route to the map</t>
-  </si>
-  <si>
-    <t>1. Initialize a map using populateMap(), stored in a Map struct variable.
-2. Initialize a Route struct variable with getBlueRoute().
-3. Initialize a Map struct with addRoute(), adding the base map and the blue route.
-4. Print the map with route using printMap().
-5. Verify results.</t>
-  </si>
-  <si>
-    <t>1. Initialize a Route struct variable with getYellowRoute().
-2. Initialize a Route struct variable with getBlueRoute().
-3. Initialize a Map struct with addRoute(), adding both routes.
-4. Print the map with route using printMap().
-5. Verify results.</t>
-  </si>
-  <si>
-    <t>Should print/display nothing since there is no base map to add routes.</t>
-  </si>
-  <si>
-    <t>Returned map should display the base map with the blue route (B symbol).</t>
-  </si>
-  <si>
-    <t>baseMap = populateMap() (get the base map)
-newRoute = getBlueRoute()
-addRoute(&amp;baseMap, &amp;newRoute)</t>
-  </si>
-  <si>
-    <t>newRoute1 = getYellowRoute()
-newRoute2 = getBlueRoute()
-addRoute(&amp;newRoute1, &amp;newRoute2)</t>
-  </si>
-  <si>
-    <t>1. Initialize a map using populateMap(), stored in a Map struct variable.
-2. Initialize a Route struct variable with getGreenRoute().
-3. Initialize a Map struct with addRoute(), adding the base map and the green route.
-4. Print the map with route using printMap().
-5. Verify results.</t>
-  </si>
-  <si>
-    <t>baseMap = populateMap() (get the base map)
-newRoute = getGreenRoute()
-addRoute(&amp;baseMap, &amp;newRoute)</t>
-  </si>
-  <si>
-    <t>1. Initialize a map using populateMap(), stored in a Map struct variable.
-2. Initialize a Route struct variable with getYellowRoute().
-3. Initialize a Map struct with addRoute(), adding the base map and the yellow route.
-4. Print the map with route using printMap().
-5. Verify results.</t>
-  </si>
-  <si>
-    <t>baseMap = populateMap() (get the base map)
-newRoute = getYellowRoute()
-addRoute(&amp;baseMap, &amp;newRoute)</t>
-  </si>
-  <si>
-    <t>Returned map should display the base map with the green route (G symbol).</t>
-  </si>
-  <si>
-    <t>Returned map should display the base map with the yellow route (Y symbol).</t>
+    <t>test_path1</t>
+  </si>
+  <si>
+    <t>Verify if the a algorithm finds the shortest path from 1A to 5E.</t>
+  </si>
+  <si>
+    <t>1. Set starting point to 1A (office location). 
+2. Set destination to 5E.  
+3. Run the algorithm to calculate the path. 
+4. Verify the calculated path.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starting Point: 1A
+Destination: 5E	</t>
+  </si>
+  <si>
+    <t>Shortest path: 1A → 2A → 3A → 4A → 5A → 5B → 5C → 5D → 5E.</t>
+  </si>
+  <si>
+    <t>test_path2</t>
+  </si>
+  <si>
+    <t>Verify if the algorithm finds the shortest path from 10K to 15P.</t>
+  </si>
+  <si>
+    <t>Starting Point: 10K
+Destination: 17L</t>
+  </si>
+  <si>
+    <t>1. Set starting point to 10K .
+2. Set destination to 17L.
+3. Run the algorithm to calculate the path.	
+4. Verify the calculated path.</t>
+  </si>
+  <si>
+    <t>Shortest path: 10K → 11K → 12K → 13K → 14K → 15K → 16K → 17K → 17L</t>
+  </si>
+  <si>
+    <t>test_path3</t>
+  </si>
+  <si>
+    <t>Verify if the algorithm detects an unreachable destination (e.g., blocked by buildings).</t>
+  </si>
+  <si>
+    <t>1. Set starting point to 6E
+2. Set destination to 2H (blocked by buildings)
+3. Run the algorithm to calculate the path.	
+4. Verify the system's response.</t>
+  </si>
+  <si>
+    <t>Destination unreachable. Package cannot be delivered / ERROR.</t>
+  </si>
+  <si>
+    <t>Starting Point: 6E
+Destination: 2H</t>
+  </si>
+  <si>
+    <t>test_path4</t>
+  </si>
+  <si>
+    <t>Verify if the algorithm handles a diversion path around a building.</t>
+  </si>
+  <si>
+    <t>Diversion path: 18V → 17V → 16V → 15V → 14V → 13V → 12V → 11V → 10V → 9V → 8V → 7V → 7W → 7X → 7Y .</t>
+  </si>
+  <si>
+    <t>Starting Point: 18v
+Destination: 7Y</t>
+  </si>
+  <si>
+    <t>1. Set starting point to 18V (blue route).
+2. Set destination to 7Y.
+3. Run the algorithm to calculate the path.
+4. Verify the calculated path.</t>
   </si>
   <si>
     <t>test_assign1</t>
@@ -646,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -672,6 +664,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -979,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="103" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,75 +1217,81 @@
       <c r="F11" s="5"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="F12" s="13"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F13" s="13"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="F14" s="13"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="B15" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
@@ -1295,80 +1303,80 @@
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
     </row>
     <row r="19" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>

</xml_diff>